<commit_message>
cleaning and rename Iy -> Iz
</commit_message>
<xml_diff>
--- a/3DBeam/output/Berechnungs_Ergebnisse.xlsx
+++ b/3DBeam/output/Berechnungs_Ergebnisse.xlsx
@@ -609,7 +609,7 @@
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Iy [m^4]</t>
+          <t>Iz [m^4]</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>Iy [m^4]</t>
+          <t>Iz [m^4]</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>Iy [m^4]</t>
+          <t>Iz [m^4]</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
@@ -681,46 +681,46 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>326.2414788463088</v>
+        <v>88.73</v>
       </c>
       <c r="E8" t="n">
-        <v>18.09557368467723</v>
+        <v>11.06</v>
       </c>
       <c r="F8" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I8" t="n">
-        <v>326.2414788463088</v>
+        <v>88.73</v>
       </c>
       <c r="J8" t="n">
-        <v>18.09557368467723</v>
+        <v>11.06</v>
       </c>
       <c r="K8" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N8" t="n">
-        <v>188.92985298382</v>
+        <v>88.73</v>
       </c>
       <c r="O8" t="n">
-        <v>15.07964473723102</v>
+        <v>11.06</v>
       </c>
       <c r="P8" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="9">
@@ -728,49 +728,49 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>13.74999973022509</v>
+        <v>13.75</v>
       </c>
       <c r="C9" t="n">
-        <v>10.925</v>
+        <v>7.42</v>
       </c>
       <c r="D9" t="n">
-        <v>246.2651736246698</v>
+        <v>70.98</v>
       </c>
       <c r="E9" t="n">
-        <v>16.47451187542489</v>
+        <v>10.26</v>
       </c>
       <c r="F9" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G9" t="n">
-        <v>13.74999973022509</v>
+        <v>13.75</v>
       </c>
       <c r="H9" t="n">
-        <v>10.5</v>
+        <v>7.3</v>
       </c>
       <c r="I9" t="n">
-        <v>218.6631801935671</v>
+        <v>67.45999999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>15.83362697409258</v>
+        <v>10.09</v>
       </c>
       <c r="K9" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L9" t="n">
-        <v>13.74999973022509</v>
+        <v>13.75</v>
       </c>
       <c r="M9" t="n">
-        <v>9.166666666666666</v>
+        <v>7.3</v>
       </c>
       <c r="N9" t="n">
-        <v>145.5876797713413</v>
+        <v>67.45999999999999</v>
       </c>
       <c r="O9" t="n">
-        <v>13.8230076757951</v>
+        <v>10.09</v>
       </c>
       <c r="P9" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="10">
@@ -778,49 +778,49 @@
         <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>27.49999946045018</v>
+        <v>27.5</v>
       </c>
       <c r="C10" t="n">
-        <v>9.85</v>
+        <v>6.85</v>
       </c>
       <c r="D10" t="n">
-        <v>180.567636742559</v>
+        <v>55.77</v>
       </c>
       <c r="E10" t="n">
-        <v>14.85345006617256</v>
+        <v>9.470000000000001</v>
       </c>
       <c r="F10" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G10" t="n">
-        <v>27.49999946045018</v>
+        <v>27.5</v>
       </c>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>6.6</v>
       </c>
       <c r="I10" t="n">
-        <v>137.8041270596067</v>
+        <v>49.9</v>
       </c>
       <c r="J10" t="n">
-        <v>13.57168026350791</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="K10" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L10" t="n">
-        <v>27.49999946045018</v>
+        <v>27.5</v>
       </c>
       <c r="M10" t="n">
-        <v>8.333333333333334</v>
+        <v>6.6</v>
       </c>
       <c r="N10" t="n">
-        <v>109.4449897233392</v>
+        <v>49.9</v>
       </c>
       <c r="O10" t="n">
-        <v>12.56637061435919</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="P10" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="11">
@@ -828,49 +828,49 @@
         <v>3</v>
       </c>
       <c r="B11" t="n">
-        <v>41.24999919067527</v>
+        <v>41.25</v>
       </c>
       <c r="C11" t="n">
-        <v>8.775</v>
+        <v>6.28</v>
       </c>
       <c r="D11" t="n">
-        <v>127.743863534989</v>
+        <v>42.9</v>
       </c>
       <c r="E11" t="n">
-        <v>13.23238825692021</v>
+        <v>8.67</v>
       </c>
       <c r="F11" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G11" t="n">
-        <v>41.24999919067527</v>
+        <v>41.25</v>
       </c>
       <c r="H11" t="n">
-        <v>7.5</v>
+        <v>5.9</v>
       </c>
       <c r="I11" t="n">
-        <v>79.8472843703159</v>
+        <v>35.68</v>
       </c>
       <c r="J11" t="n">
-        <v>11.30973355292327</v>
+        <v>8.16</v>
       </c>
       <c r="K11" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L11" t="n">
-        <v>41.24999919067527</v>
+        <v>41.25</v>
       </c>
       <c r="M11" t="n">
-        <v>7.5</v>
+        <v>5.9</v>
       </c>
       <c r="N11" t="n">
-        <v>79.8472843703159</v>
+        <v>35.68</v>
       </c>
       <c r="O11" t="n">
-        <v>11.30973355292327</v>
+        <v>8.16</v>
       </c>
       <c r="P11" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="12">
@@ -878,49 +878,49 @@
         <v>4</v>
       </c>
       <c r="B12" t="n">
-        <v>54.99999892090035</v>
+        <v>55</v>
       </c>
       <c r="C12" t="n">
-        <v>7.7</v>
+        <v>5.7</v>
       </c>
       <c r="D12" t="n">
-        <v>86.38884933697129</v>
+        <v>32.19</v>
       </c>
       <c r="E12" t="n">
-        <v>11.61132644766786</v>
+        <v>7.88</v>
       </c>
       <c r="F12" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G12" t="n">
-        <v>54.99999892090035</v>
+        <v>55</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="I12" t="n">
-        <v>40.97561705158311</v>
+        <v>24.47</v>
       </c>
       <c r="J12" t="n">
-        <v>9.047786842338613</v>
+        <v>7.19</v>
       </c>
       <c r="K12" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L12" t="n">
-        <v>54.99999892090035</v>
+        <v>55</v>
       </c>
       <c r="M12" t="n">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="N12" t="n">
-        <v>40.97561705158311</v>
+        <v>24.47</v>
       </c>
       <c r="O12" t="n">
-        <v>9.047786842338613</v>
+        <v>7.19</v>
       </c>
       <c r="P12" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="13">
@@ -928,49 +928,49 @@
         <v>5</v>
       </c>
       <c r="B13" t="n">
-        <v>68.74999865112544</v>
+        <v>68.75</v>
       </c>
       <c r="C13" t="n">
-        <v>6.625</v>
+        <v>5.12</v>
       </c>
       <c r="D13" t="n">
-        <v>55.09758948351856</v>
+        <v>23.43</v>
       </c>
       <c r="E13" t="n">
-        <v>9.99026463841555</v>
+        <v>7.08</v>
       </c>
       <c r="F13" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G13" t="n">
-        <v>68.74999865112544</v>
+        <v>68.75</v>
       </c>
       <c r="H13" t="n">
-        <v>5.35</v>
+        <v>4.5</v>
       </c>
       <c r="I13" t="n">
-        <v>29.09674283459829</v>
+        <v>15.9</v>
       </c>
       <c r="J13" t="n">
-        <v>8.067609934418595</v>
+        <v>6.22</v>
       </c>
       <c r="K13" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L13" t="n">
-        <v>68.74999865112544</v>
+        <v>68.75</v>
       </c>
       <c r="M13" t="n">
-        <v>5.35</v>
+        <v>4.5</v>
       </c>
       <c r="N13" t="n">
-        <v>29.09674283459829</v>
+        <v>15.9</v>
       </c>
       <c r="O13" t="n">
-        <v>8.067609934418595</v>
+        <v>6.22</v>
       </c>
       <c r="P13" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="14">
@@ -978,49 +978,49 @@
         <v>6</v>
       </c>
       <c r="B14" t="n">
-        <v>82.49999838135054</v>
+        <v>82.5</v>
       </c>
       <c r="C14" t="n">
-        <v>5.550000000000001</v>
+        <v>4.55</v>
       </c>
       <c r="D14" t="n">
-        <v>32.46507930964241</v>
+        <v>16.43</v>
       </c>
       <c r="E14" t="n">
-        <v>8.369202829163218</v>
+        <v>6.29</v>
       </c>
       <c r="F14" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G14" t="n">
-        <v>82.49999838135054</v>
+        <v>82.5</v>
       </c>
       <c r="H14" t="n">
-        <v>4.7</v>
+        <v>4.13</v>
       </c>
       <c r="I14" t="n">
-        <v>19.77429251558233</v>
+        <v>12.34</v>
       </c>
       <c r="J14" t="n">
-        <v>7.087433026498564</v>
+        <v>5.71</v>
       </c>
       <c r="K14" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L14" t="n">
-        <v>82.49999838135054</v>
+        <v>82.5</v>
       </c>
       <c r="M14" t="n">
-        <v>4.7</v>
+        <v>4.13</v>
       </c>
       <c r="N14" t="n">
-        <v>19.77429251558233</v>
+        <v>12.34</v>
       </c>
       <c r="O14" t="n">
-        <v>7.087433026498564</v>
+        <v>5.71</v>
       </c>
       <c r="P14" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="15">
@@ -1028,49 +1028,49 @@
         <v>7</v>
       </c>
       <c r="B15" t="n">
-        <v>96.24999811157562</v>
+        <v>96.25</v>
       </c>
       <c r="C15" t="n">
-        <v>4.475000000000001</v>
+        <v>3.98</v>
       </c>
       <c r="D15" t="n">
-        <v>17.08631415035502</v>
+        <v>10.99</v>
       </c>
       <c r="E15" t="n">
-        <v>6.74814101991087</v>
+        <v>5.49</v>
       </c>
       <c r="F15" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G15" t="n">
-        <v>96.24999811157562</v>
+        <v>96.25</v>
       </c>
       <c r="H15" t="n">
-        <v>4.05</v>
+        <v>3.77</v>
       </c>
       <c r="I15" t="n">
-        <v>12.69767253683815</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>6.107256118578555</v>
+        <v>5.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L15" t="n">
-        <v>96.24999811157562</v>
+        <v>96.25</v>
       </c>
       <c r="M15" t="n">
-        <v>4.05</v>
+        <v>3.77</v>
       </c>
       <c r="N15" t="n">
-        <v>12.69767253683815</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="O15" t="n">
-        <v>6.107256118578555</v>
+        <v>5.21</v>
       </c>
       <c r="P15" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="16">
@@ -1078,49 +1078,49 @@
         <v>8</v>
       </c>
       <c r="B16" t="n">
-        <v>109.9999978418007</v>
+        <v>110</v>
       </c>
       <c r="C16" t="n">
         <v>3.4</v>
       </c>
       <c r="D16" t="n">
-        <v>7.55628934066856</v>
+        <v>6.9</v>
       </c>
       <c r="E16" t="n">
-        <v>5.127079210658543</v>
+        <v>4.7</v>
       </c>
       <c r="F16" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="G16" t="n">
-        <v>109.9999978418007</v>
+        <v>110</v>
       </c>
       <c r="H16" t="n">
         <v>3.4</v>
       </c>
       <c r="I16" t="n">
-        <v>7.55628934066856</v>
+        <v>6.9</v>
       </c>
       <c r="J16" t="n">
-        <v>5.127079210658543</v>
+        <v>4.7</v>
       </c>
       <c r="K16" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="L16" t="n">
-        <v>109.9999978418007</v>
+        <v>110</v>
       </c>
       <c r="M16" t="n">
         <v>3.4</v>
       </c>
       <c r="N16" t="n">
-        <v>7.55628934066856</v>
+        <v>6.9</v>
       </c>
       <c r="O16" t="n">
-        <v>5.127079210658543</v>
+        <v>4.7</v>
       </c>
       <c r="P16" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -1195,6 +1195,11 @@
           <t>cd</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cp_max</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1203,7 +1208,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.48</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>110</v>
@@ -1211,6 +1216,9 @@
       <c r="D2" t="n">
         <v>1.1</v>
       </c>
+      <c r="E2" t="n">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1219,7 +1227,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.48</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="C3" t="n">
         <v>110</v>
@@ -1227,6 +1235,9 @@
       <c r="D3" t="n">
         <v>1.1</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1235,13 +1246,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.48</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="C4" t="n">
         <v>110</v>
       </c>
       <c r="D4" t="n">
         <v>1.1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="6">
@@ -1455,73 +1469,73 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>2.49</v>
+        <v>6.77</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.24</v>
+        <v>-15.15</v>
       </c>
       <c r="E10" t="n">
-        <v>46.88</v>
+        <v>78.94</v>
       </c>
       <c r="F10" t="n">
-        <v>0.401</v>
+        <v>0.89</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="I10" t="n">
-        <v>0.22</v>
+        <v>0.35</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2.53</v>
+        <v>6.79</v>
       </c>
       <c r="L10" t="n">
-        <v>-6.24</v>
+        <v>-15.14</v>
       </c>
       <c r="M10" t="n">
-        <v>47.7</v>
+        <v>79.2</v>
       </c>
       <c r="N10" t="n">
-        <v>0.4</v>
+        <v>0.889</v>
       </c>
       <c r="O10" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="P10" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.22</v>
+        <v>0.35</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>3.85</v>
+        <v>6.79</v>
       </c>
       <c r="T10" t="n">
-        <v>-9.039999999999999</v>
+        <v>-15.14</v>
       </c>
       <c r="U10" t="n">
-        <v>60.78</v>
+        <v>79.2</v>
       </c>
       <c r="V10" t="n">
-        <v>0.58</v>
+        <v>0.889</v>
       </c>
       <c r="W10" t="n">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="X10" t="n">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="11">
@@ -1532,73 +1546,73 @@
         <v>13.75</v>
       </c>
       <c r="C11" t="n">
-        <v>2.62</v>
+        <v>6.79</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.46</v>
+        <v>-15.14</v>
       </c>
       <c r="E11" t="n">
-        <v>45.1</v>
+        <v>73.8</v>
       </c>
       <c r="F11" t="n">
-        <v>0.414</v>
+        <v>0.889</v>
       </c>
       <c r="G11" t="n">
-        <v>0.21</v>
+        <v>0.32</v>
       </c>
       <c r="H11" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="I11" t="n">
-        <v>0.24</v>
+        <v>0.38</v>
       </c>
       <c r="J11" t="n">
         <v>13.75</v>
       </c>
       <c r="K11" t="n">
-        <v>2.92</v>
+        <v>7.07</v>
       </c>
       <c r="L11" t="n">
-        <v>-6.99</v>
+        <v>-15.67</v>
       </c>
       <c r="M11" t="n">
-        <v>48.33</v>
+        <v>75.62</v>
       </c>
       <c r="N11" t="n">
-        <v>0.448</v>
+        <v>0.92</v>
       </c>
       <c r="O11" t="n">
-        <v>0.22</v>
+        <v>0.32</v>
       </c>
       <c r="P11" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.25</v>
+        <v>0.39</v>
       </c>
       <c r="R11" t="n">
         <v>13.75</v>
       </c>
       <c r="S11" t="n">
-        <v>3.96</v>
+        <v>7.07</v>
       </c>
       <c r="T11" t="n">
-        <v>-9.23</v>
+        <v>-15.67</v>
       </c>
       <c r="U11" t="n">
-        <v>57.66</v>
+        <v>75.62</v>
       </c>
       <c r="V11" t="n">
-        <v>0.591</v>
+        <v>0.92</v>
       </c>
       <c r="W11" t="n">
-        <v>0.25</v>
+        <v>0.32</v>
       </c>
       <c r="X11" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.29</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="12">
@@ -1609,73 +1623,73 @@
         <v>27.5</v>
       </c>
       <c r="C12" t="n">
-        <v>2.75</v>
+        <v>6.75</v>
       </c>
       <c r="D12" t="n">
-        <v>-6.68</v>
+        <v>-15.03</v>
       </c>
       <c r="E12" t="n">
-        <v>42.91</v>
+        <v>68.04000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>0.428</v>
+        <v>0.882</v>
       </c>
       <c r="G12" t="n">
-        <v>0.22</v>
+        <v>0.33</v>
       </c>
       <c r="H12" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I12" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="J12" t="n">
         <v>27.5</v>
       </c>
       <c r="K12" t="n">
-        <v>3.43</v>
+        <v>7.35</v>
       </c>
       <c r="L12" t="n">
-        <v>-8.02</v>
+        <v>-16.21</v>
       </c>
       <c r="M12" t="n">
-        <v>49</v>
+        <v>71.48</v>
       </c>
       <c r="N12" t="n">
-        <v>0.514</v>
+        <v>0.952</v>
       </c>
       <c r="O12" t="n">
-        <v>0.24</v>
+        <v>0.34</v>
       </c>
       <c r="P12" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.28</v>
+        <v>0.42</v>
       </c>
       <c r="R12" t="n">
         <v>27.5</v>
       </c>
       <c r="S12" t="n">
-        <v>4.07</v>
+        <v>7.35</v>
       </c>
       <c r="T12" t="n">
-        <v>-9.390000000000001</v>
+        <v>-16.21</v>
       </c>
       <c r="U12" t="n">
-        <v>54.07</v>
+        <v>71.48</v>
       </c>
       <c r="V12" t="n">
-        <v>0.602</v>
+        <v>0.952</v>
       </c>
       <c r="W12" t="n">
-        <v>0.26</v>
+        <v>0.34</v>
       </c>
       <c r="X12" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.31</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="13">
@@ -1686,73 +1700,73 @@
         <v>41.25</v>
       </c>
       <c r="C13" t="n">
-        <v>2.88</v>
+        <v>6.63</v>
       </c>
       <c r="D13" t="n">
-        <v>-6.9</v>
+        <v>-14.74</v>
       </c>
       <c r="E13" t="n">
-        <v>40.24</v>
+        <v>61.53</v>
       </c>
       <c r="F13" t="n">
-        <v>0.442</v>
+        <v>0.865</v>
       </c>
       <c r="G13" t="n">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
       <c r="H13" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="I13" t="n">
-        <v>0.28</v>
+        <v>0.43</v>
       </c>
       <c r="J13" t="n">
         <v>41.25</v>
       </c>
       <c r="K13" t="n">
-        <v>4.15</v>
+        <v>7.6</v>
       </c>
       <c r="L13" t="n">
-        <v>-9.51</v>
+        <v>-16.73</v>
       </c>
       <c r="M13" t="n">
-        <v>49.91</v>
+        <v>66.63</v>
       </c>
       <c r="N13" t="n">
-        <v>0.609</v>
+        <v>0.982</v>
       </c>
       <c r="O13" t="n">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
       <c r="P13" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.33</v>
+        <v>0.46</v>
       </c>
       <c r="R13" t="n">
         <v>41.25</v>
       </c>
       <c r="S13" t="n">
-        <v>4.15</v>
+        <v>7.6</v>
       </c>
       <c r="T13" t="n">
-        <v>-9.51</v>
+        <v>-16.73</v>
       </c>
       <c r="U13" t="n">
-        <v>49.91</v>
+        <v>66.63</v>
       </c>
       <c r="V13" t="n">
-        <v>0.609</v>
+        <v>0.982</v>
       </c>
       <c r="W13" t="n">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
       <c r="X13" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.33</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="14">
@@ -1763,73 +1777,73 @@
         <v>55</v>
       </c>
       <c r="C14" t="n">
-        <v>2.99</v>
+        <v>6.36</v>
       </c>
       <c r="D14" t="n">
-        <v>-7.09</v>
+        <v>-14.19</v>
       </c>
       <c r="E14" t="n">
-        <v>36.9</v>
+        <v>54.01</v>
       </c>
       <c r="F14" t="n">
-        <v>0.454</v>
+        <v>0.832</v>
       </c>
       <c r="G14" t="n">
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="H14" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3</v>
+        <v>0.47</v>
       </c>
       <c r="J14" t="n">
         <v>55</v>
       </c>
       <c r="K14" t="n">
-        <v>5.26</v>
+        <v>7.79</v>
       </c>
       <c r="L14" t="n">
-        <v>-11.84</v>
+        <v>-17.14</v>
       </c>
       <c r="M14" t="n">
-        <v>51.37</v>
+        <v>60.76</v>
       </c>
       <c r="N14" t="n">
-        <v>0.758</v>
+        <v>1.005</v>
       </c>
       <c r="O14" t="n">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="P14" t="n">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.41</v>
+        <v>0.52</v>
       </c>
       <c r="R14" t="n">
         <v>55</v>
       </c>
       <c r="S14" t="n">
-        <v>5.26</v>
+        <v>7.79</v>
       </c>
       <c r="T14" t="n">
-        <v>-11.84</v>
+        <v>-17.14</v>
       </c>
       <c r="U14" t="n">
-        <v>51.37</v>
+        <v>60.76</v>
       </c>
       <c r="V14" t="n">
-        <v>0.758</v>
+        <v>1.005</v>
       </c>
       <c r="W14" t="n">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="X14" t="n">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.41</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="15">
@@ -1840,73 +1854,73 @@
         <v>68.75</v>
       </c>
       <c r="C15" t="n">
-        <v>3.03</v>
+        <v>5.86</v>
       </c>
       <c r="D15" t="n">
-        <v>-7.18</v>
+        <v>-13.16</v>
       </c>
       <c r="E15" t="n">
-        <v>32.5</v>
+        <v>45.07</v>
       </c>
       <c r="F15" t="n">
-        <v>0.459</v>
+        <v>0.772</v>
       </c>
       <c r="G15" t="n">
-        <v>0.28</v>
+        <v>0.39</v>
       </c>
       <c r="H15" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="I15" t="n">
-        <v>0.35</v>
+        <v>0.51</v>
       </c>
       <c r="J15" t="n">
         <v>68.75</v>
       </c>
       <c r="K15" t="n">
-        <v>4.92</v>
+        <v>7.81</v>
       </c>
       <c r="L15" t="n">
-        <v>-11.15</v>
+        <v>-17.22</v>
       </c>
       <c r="M15" t="n">
-        <v>43.23</v>
+        <v>53.3</v>
       </c>
       <c r="N15" t="n">
-        <v>0.713</v>
+        <v>1.01</v>
       </c>
       <c r="O15" t="n">
-        <v>0.34</v>
+        <v>0.44</v>
       </c>
       <c r="P15" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="R15" t="n">
         <v>68.75</v>
       </c>
       <c r="S15" t="n">
-        <v>4.92</v>
+        <v>7.81</v>
       </c>
       <c r="T15" t="n">
-        <v>-11.15</v>
+        <v>-17.22</v>
       </c>
       <c r="U15" t="n">
-        <v>43.23</v>
+        <v>53.3</v>
       </c>
       <c r="V15" t="n">
-        <v>0.713</v>
+        <v>1.01</v>
       </c>
       <c r="W15" t="n">
-        <v>0.34</v>
+        <v>0.44</v>
       </c>
       <c r="X15" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16">
@@ -1917,73 +1931,73 @@
         <v>82.5</v>
       </c>
       <c r="C16" t="n">
-        <v>2.9</v>
+        <v>4.94</v>
       </c>
       <c r="D16" t="n">
-        <v>-6.93</v>
+        <v>-11.32</v>
       </c>
       <c r="E16" t="n">
-        <v>26.35</v>
+        <v>34.05</v>
       </c>
       <c r="F16" t="n">
-        <v>0.443</v>
+        <v>0.664</v>
       </c>
       <c r="G16" t="n">
-        <v>0.32</v>
+        <v>0.42</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="I16" t="n">
-        <v>0.42</v>
+        <v>0.58</v>
       </c>
       <c r="J16" t="n">
         <v>82.5</v>
       </c>
       <c r="K16" t="n">
-        <v>4.23</v>
+        <v>6.12</v>
       </c>
       <c r="L16" t="n">
-        <v>-9.779999999999999</v>
+        <v>-13.82</v>
       </c>
       <c r="M16" t="n">
-        <v>33.06</v>
+        <v>38.68</v>
       </c>
       <c r="N16" t="n">
-        <v>0.625</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="O16" t="n">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
       <c r="P16" t="n">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.51</v>
+        <v>0.65</v>
       </c>
       <c r="R16" t="n">
         <v>82.5</v>
       </c>
       <c r="S16" t="n">
-        <v>4.23</v>
+        <v>6.12</v>
       </c>
       <c r="T16" t="n">
-        <v>-9.779999999999999</v>
+        <v>-13.82</v>
       </c>
       <c r="U16" t="n">
-        <v>33.06</v>
+        <v>38.68</v>
       </c>
       <c r="V16" t="n">
-        <v>0.625</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="W16" t="n">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
       <c r="X16" t="n">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.51</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="17">
@@ -1994,73 +2008,73 @@
         <v>96.25</v>
       </c>
       <c r="C17" t="n">
-        <v>2.27</v>
+        <v>3.26</v>
       </c>
       <c r="D17" t="n">
-        <v>-5.77</v>
+        <v>-8</v>
       </c>
       <c r="E17" t="n">
-        <v>16.98</v>
+        <v>19.89</v>
       </c>
       <c r="F17" t="n">
-        <v>0.369</v>
+        <v>0.468</v>
       </c>
       <c r="G17" t="n">
-        <v>0.37</v>
+        <v>0.45</v>
       </c>
       <c r="H17" t="n">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="I17" t="n">
-        <v>0.52</v>
+        <v>0.67</v>
       </c>
       <c r="J17" t="n">
         <v>96.25</v>
       </c>
       <c r="K17" t="n">
-        <v>2.88</v>
+        <v>3.69</v>
       </c>
       <c r="L17" t="n">
-        <v>-7.1</v>
+        <v>-8.94</v>
       </c>
       <c r="M17" t="n">
-        <v>19.65</v>
+        <v>21.47</v>
       </c>
       <c r="N17" t="n">
-        <v>0.454</v>
+        <v>0.524</v>
       </c>
       <c r="O17" t="n">
-        <v>0.41</v>
+        <v>0.48</v>
       </c>
       <c r="P17" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.6</v>
+        <v>0.71</v>
       </c>
       <c r="R17" t="n">
         <v>96.25</v>
       </c>
       <c r="S17" t="n">
-        <v>2.88</v>
+        <v>3.69</v>
       </c>
       <c r="T17" t="n">
-        <v>-7.1</v>
+        <v>-8.94</v>
       </c>
       <c r="U17" t="n">
-        <v>19.65</v>
+        <v>21.47</v>
       </c>
       <c r="V17" t="n">
-        <v>0.454</v>
+        <v>0.524</v>
       </c>
       <c r="W17" t="n">
-        <v>0.41</v>
+        <v>0.48</v>
       </c>
       <c r="X17" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.6</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="18">
@@ -2071,73 +2085,73 @@
         <v>110</v>
       </c>
       <c r="C18" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.66</v>
+        <v>-1.8</v>
       </c>
       <c r="E18" t="n">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="F18" t="n">
-        <v>0.106</v>
+        <v>0.105</v>
       </c>
       <c r="G18" t="n">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
       <c r="H18" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="I18" t="n">
-        <v>0.73</v>
+        <v>0.8</v>
       </c>
       <c r="J18" t="n">
         <v>110</v>
       </c>
       <c r="K18" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="L18" t="n">
-        <v>-1.66</v>
+        <v>-1.8</v>
       </c>
       <c r="M18" t="n">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="N18" t="n">
-        <v>0.106</v>
+        <v>0.105</v>
       </c>
       <c r="O18" t="n">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
       <c r="P18" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.73</v>
+        <v>0.8</v>
       </c>
       <c r="R18" t="n">
         <v>110</v>
       </c>
       <c r="S18" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="T18" t="n">
-        <v>-1.66</v>
+        <v>-1.8</v>
       </c>
       <c r="U18" t="n">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="V18" t="n">
-        <v>0.106</v>
+        <v>0.105</v>
       </c>
       <c r="W18" t="n">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
       <c r="X18" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.73</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -2201,7 +2215,7 @@
     <row r="1">
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>t, tX, tY [cm] 48, 40.0, 8.0</t>
+          <t>t, tX, tY [cm] 44, 40.0, 4.0</t>
         </is>
       </c>
     </row>
@@ -2229,13 +2243,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4591390637970857</v>
+        <v>0.8900077810999515</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7580634707275777</v>
+        <v>1.00997902899666</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7580634707276442</v>
+        <v>1.00997902899666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auswertung  an Ebenen und FE Knoten
</commit_message>
<xml_diff>
--- a/3DBeam/output/Berechnungs_Ergebnisse.xlsx
+++ b/3DBeam/output/Berechnungs_Ergebnisse.xlsx
@@ -480,6 +480,7 @@
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -634,14 +635,15 @@
       <c r="A5" s="1" t="inlineStr"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
       <c r="C5" s="2" t="n"/>
       <c r="D5" s="2" t="n"/>
       <c r="E5" s="2" t="n"/>
       <c r="F5" s="2" t="n"/>
-      <c r="G5" s="3" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="3" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr"/>
@@ -675,6 +677,11 @@
           <t>t [m]</t>
         </is>
       </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>V_section [m³]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -697,6 +704,9 @@
       </c>
       <c r="G8" t="n">
         <v>0.36</v>
+      </c>
+      <c r="H8" t="n">
+        <v>170.88</v>
       </c>
     </row>
     <row r="9">
@@ -721,6 +731,9 @@
       <c r="G9" t="n">
         <v>0.36</v>
       </c>
+      <c r="H9" t="n">
+        <v>157.24</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -744,6 +757,9 @@
       <c r="G10" t="n">
         <v>0.36</v>
       </c>
+      <c r="H10" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -767,6 +783,9 @@
       <c r="G11" t="n">
         <v>0.36</v>
       </c>
+      <c r="H11" t="n">
+        <v>129.96</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -790,6 +809,9 @@
       <c r="G12" t="n">
         <v>0.36</v>
       </c>
+      <c r="H12" t="n">
+        <v>116.31</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -813,6 +835,9 @@
       <c r="G13" t="n">
         <v>0.36</v>
       </c>
+      <c r="H13" t="n">
+        <v>102.67</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -836,6 +861,9 @@
       <c r="G14" t="n">
         <v>0.36</v>
       </c>
+      <c r="H14" t="n">
+        <v>89.03</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -859,6 +887,9 @@
       <c r="G15" t="n">
         <v>0.36</v>
       </c>
+      <c r="H15" t="n">
+        <v>75.39</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -882,6 +913,9 @@
       <c r="G16" t="n">
         <v>0.36</v>
       </c>
+      <c r="H16" t="n">
+        <v>61.75</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -905,10 +939,13 @@
       <c r="G17" t="n">
         <v>0.36</v>
       </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1046,7 +1083,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
       <c r="C6" s="2" t="n"/>
@@ -1981,7 +2018,7 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
       <c r="C35" s="2" t="n"/>
@@ -2672,7 +2709,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
       <c r="C6" s="2" t="n"/>
@@ -2738,7 +2775,7 @@
         <v>86.90000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>4</v>
@@ -2764,7 +2801,7 @@
         <v>82.09999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -2790,7 +2827,7 @@
         <v>76.90000000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>5</v>
@@ -2816,7 +2853,7 @@
         <v>71.2</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>6</v>
@@ -2842,7 +2879,7 @@
         <v>64.90000000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>6</v>
@@ -2868,7 +2905,7 @@
         <v>57.7</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>8</v>
@@ -2894,7 +2931,7 @@
         <v>49.1</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2920,7 +2957,7 @@
         <v>38.4</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2946,7 +2983,7 @@
         <v>23.9</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -2999,7 +3036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3026,6 +3063,7 @@
     <col width="17" customWidth="1" min="17" max="17"/>
     <col width="17" customWidth="1" min="18" max="18"/>
     <col width="17" customWidth="1" min="19" max="19"/>
+    <col width="17" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3058,7 +3096,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -3099,7 +3137,8 @@
       <c r="P4" s="2" t="n"/>
       <c r="Q4" s="2" t="n"/>
       <c r="R4" s="2" t="n"/>
-      <c r="S4" s="3" t="n"/>
+      <c r="S4" s="2" t="n"/>
+      <c r="T4" s="3" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -3109,7 +3148,7 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
       <c r="C5" s="2" t="n"/>
@@ -3128,7 +3167,8 @@
       <c r="P5" s="2" t="n"/>
       <c r="Q5" s="2" t="n"/>
       <c r="R5" s="2" t="n"/>
-      <c r="S5" s="3" t="n"/>
+      <c r="S5" s="2" t="n"/>
+      <c r="T5" s="3" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -3153,75 +3193,80 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
+          <t>P_ist [MN]</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
           <t>M [MNm]</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="G6" s="1" t="inlineStr">
         <is>
           <t>N [MN]</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t>Q [MN]</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>σ_druck [N/mm²]</t>
-        </is>
-      </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
+          <t>σ_min [N/mm²]</t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
           <t>Ausn. druck</t>
         </is>
       </c>
-      <c r="J6" s="1" t="inlineStr">
+      <c r="K6" s="1" t="inlineStr">
         <is>
           <t>τ_Fe [N/mm²]</t>
         </is>
       </c>
-      <c r="K6" s="1" t="inlineStr">
+      <c r="L6" s="1" t="inlineStr">
         <is>
           <t>τ_längs [N/mm²]</t>
         </is>
       </c>
-      <c r="L6" s="1" t="inlineStr">
+      <c r="M6" s="1" t="inlineStr">
         <is>
           <t>Ausn. schub Furnier</t>
         </is>
       </c>
-      <c r="M6" s="1" t="inlineStr">
+      <c r="N6" s="1" t="inlineStr">
         <is>
           <t>Ausn. schub längs</t>
         </is>
       </c>
-      <c r="N6" s="1" t="inlineStr">
+      <c r="O6" s="1" t="inlineStr">
         <is>
           <t>nxy_Qy [kN/m]</t>
         </is>
       </c>
-      <c r="O6" s="1" t="inlineStr">
+      <c r="P6" s="1" t="inlineStr">
         <is>
           <t>nxy_Mx [kNm/m]</t>
         </is>
       </c>
-      <c r="P6" s="1" t="inlineStr">
-        <is>
-          <t>nxy_P [kN/m]</t>
-        </is>
-      </c>
       <c r="Q6" s="1" t="inlineStr">
         <is>
+          <t>nxy_P,Rd [kN/m]</t>
+        </is>
+      </c>
+      <c r="R6" s="1" t="inlineStr">
+        <is>
           <t>Ausn. reibung</t>
         </is>
       </c>
-      <c r="R6" s="1" t="inlineStr">
+      <c r="S6" s="1" t="inlineStr">
         <is>
           <t>fvd_Fe</t>
         </is>
       </c>
-      <c r="S6" s="1" t="inlineStr">
+      <c r="T6" s="1" t="inlineStr">
         <is>
           <t>fvd_längs</t>
         </is>
@@ -3241,48 +3286,51 @@
         <v>86.84999999999999</v>
       </c>
       <c r="E8" t="n">
+        <v>87.12</v>
+      </c>
+      <c r="F8" t="n">
         <v>-206.94</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>-10.21</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>2</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>-14</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.964</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>3.3</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>0.39</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.12</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>0.11</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>363.35</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>12.15</v>
       </c>
-      <c r="P8" t="n">
-        <v>1256.66</v>
-      </c>
       <c r="Q8" t="n">
-        <v>0.299</v>
+        <v>1260.48</v>
       </c>
       <c r="R8" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="S8" t="n">
         <v>27.9</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3291,57 +3339,60 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>14.44</v>
+        <v>6.5</v>
       </c>
       <c r="C9" t="n">
-        <v>10.16</v>
+        <v>10.62</v>
       </c>
       <c r="D9" t="n">
-        <v>82.06999999999999</v>
+        <v>86.84999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>-178.74</v>
+        <v>87.12</v>
       </c>
       <c r="F9" t="n">
-        <v>-9.140000000000001</v>
+        <v>-194.08</v>
       </c>
       <c r="G9" t="n">
-        <v>1.93</v>
+        <v>-9.720000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>-14.25</v>
+        <v>1.98</v>
       </c>
       <c r="I9" t="n">
-        <v>0.981</v>
+        <v>-14.27</v>
       </c>
       <c r="J9" t="n">
-        <v>3.47</v>
+        <v>0.985</v>
       </c>
       <c r="K9" t="n">
-        <v>0.41</v>
+        <v>3.39</v>
       </c>
       <c r="L9" t="n">
-        <v>0.127</v>
+        <v>0.4</v>
       </c>
       <c r="M9" t="n">
-        <v>0.116</v>
+        <v>0.124</v>
       </c>
       <c r="N9" t="n">
-        <v>380.01</v>
+        <v>0.113</v>
       </c>
       <c r="O9" t="n">
-        <v>14.26</v>
+        <v>372.54</v>
       </c>
       <c r="P9" t="n">
-        <v>1286.19</v>
+        <v>13.04</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.307</v>
+        <v>1305.58</v>
       </c>
       <c r="R9" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="S9" t="n">
         <v>27.9</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3350,57 +3401,60 @@
         <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>28.89</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>9.31</v>
+        <v>10.24</v>
       </c>
       <c r="D10" t="n">
-        <v>76.86</v>
+        <v>86.84999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>-151.92</v>
+        <v>87.12</v>
       </c>
       <c r="F10" t="n">
-        <v>-8.15</v>
+        <v>-181.47</v>
       </c>
       <c r="G10" t="n">
-        <v>1.83</v>
+        <v>-9.24</v>
       </c>
       <c r="H10" t="n">
-        <v>-14.42</v>
+        <v>1.94</v>
       </c>
       <c r="I10" t="n">
-        <v>0.992</v>
+        <v>-14.56</v>
       </c>
       <c r="J10" t="n">
-        <v>3.62</v>
+        <v>1.006</v>
       </c>
       <c r="K10" t="n">
-        <v>0.43</v>
+        <v>3.45</v>
       </c>
       <c r="L10" t="n">
-        <v>0.132</v>
+        <v>0.41</v>
       </c>
       <c r="M10" t="n">
-        <v>0.121</v>
+        <v>0.126</v>
       </c>
       <c r="N10" t="n">
-        <v>392.84</v>
+        <v>0.116</v>
       </c>
       <c r="O10" t="n">
-        <v>16.96</v>
+        <v>378.77</v>
       </c>
       <c r="P10" t="n">
-        <v>1313.73</v>
+        <v>14.02</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.312</v>
+        <v>1354.03</v>
       </c>
       <c r="R10" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="S10" t="n">
         <v>27.9</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3409,57 +3463,60 @@
         <v>3</v>
       </c>
       <c r="B11" t="n">
-        <v>43.33</v>
+        <v>19.5</v>
       </c>
       <c r="C11" t="n">
-        <v>8.470000000000001</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="D11" t="n">
-        <v>71.17</v>
+        <v>82.06999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>-126.6</v>
+        <v>82.69</v>
       </c>
       <c r="F11" t="n">
-        <v>-7.25</v>
+        <v>-169.15</v>
       </c>
       <c r="G11" t="n">
-        <v>1.72</v>
+        <v>-8.779999999999999</v>
       </c>
       <c r="H11" t="n">
-        <v>-14.59</v>
+        <v>1.9</v>
       </c>
       <c r="I11" t="n">
-        <v>1.005</v>
+        <v>-14.47</v>
       </c>
       <c r="J11" t="n">
-        <v>3.79</v>
+        <v>0.999</v>
       </c>
       <c r="K11" t="n">
-        <v>0.45</v>
+        <v>3.52</v>
       </c>
       <c r="L11" t="n">
-        <v>0.138</v>
+        <v>0.42</v>
       </c>
       <c r="M11" t="n">
-        <v>0.126</v>
+        <v>0.128</v>
       </c>
       <c r="N11" t="n">
-        <v>407.18</v>
+        <v>0.118</v>
       </c>
       <c r="O11" t="n">
-        <v>20.51</v>
+        <v>384.52</v>
       </c>
       <c r="P11" t="n">
-        <v>1337.79</v>
+        <v>15.13</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.32</v>
+        <v>1334.74</v>
       </c>
       <c r="R11" t="n">
+        <v>0.299</v>
+      </c>
+      <c r="S11" t="n">
         <v>27.9</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3468,57 +3525,60 @@
         <v>4</v>
       </c>
       <c r="B12" t="n">
-        <v>57.78</v>
+        <v>26</v>
       </c>
       <c r="C12" t="n">
-        <v>7.62</v>
+        <v>9.48</v>
       </c>
       <c r="D12" t="n">
-        <v>64.84999999999999</v>
+        <v>82.06999999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>-102.77</v>
+        <v>82.69</v>
       </c>
       <c r="F12" t="n">
-        <v>-6.43</v>
+        <v>-157.13</v>
       </c>
       <c r="G12" t="n">
-        <v>1.62</v>
+        <v>-8.34</v>
       </c>
       <c r="H12" t="n">
-        <v>-14.64</v>
+        <v>1.85</v>
       </c>
       <c r="I12" t="n">
-        <v>1.007</v>
+        <v>-14.78</v>
       </c>
       <c r="J12" t="n">
-        <v>4.01</v>
+        <v>1.022</v>
       </c>
       <c r="K12" t="n">
-        <v>0.47</v>
+        <v>3.59</v>
       </c>
       <c r="L12" t="n">
-        <v>0.146</v>
+        <v>0.42</v>
       </c>
       <c r="M12" t="n">
-        <v>0.134</v>
+        <v>0.131</v>
       </c>
       <c r="N12" t="n">
-        <v>425.08</v>
+        <v>0.12</v>
       </c>
       <c r="O12" t="n">
-        <v>25.31</v>
+        <v>390.25</v>
       </c>
       <c r="P12" t="n">
-        <v>1354.11</v>
+        <v>16.36</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.333</v>
+        <v>1388.24</v>
       </c>
       <c r="R12" t="n">
+        <v>0.293</v>
+      </c>
+      <c r="S12" t="n">
         <v>27.9</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3527,57 +3587,60 @@
         <v>5</v>
       </c>
       <c r="B13" t="n">
-        <v>72.22</v>
+        <v>32.5</v>
       </c>
       <c r="C13" t="n">
-        <v>6.78</v>
+        <v>9.1</v>
       </c>
       <c r="D13" t="n">
-        <v>57.66</v>
+        <v>76.86</v>
       </c>
       <c r="E13" t="n">
-        <v>-80.41</v>
+        <v>77.16</v>
       </c>
       <c r="F13" t="n">
-        <v>-5.7</v>
+        <v>-145.41</v>
       </c>
       <c r="G13" t="n">
-        <v>1.52</v>
+        <v>-7.92</v>
       </c>
       <c r="H13" t="n">
-        <v>-14.64</v>
+        <v>1.8</v>
       </c>
       <c r="I13" t="n">
-        <v>1.007</v>
+        <v>-14.59</v>
       </c>
       <c r="J13" t="n">
-        <v>4.3</v>
+        <v>1.006</v>
       </c>
       <c r="K13" t="n">
-        <v>0.51</v>
+        <v>3.66</v>
       </c>
       <c r="L13" t="n">
-        <v>0.156</v>
+        <v>0.43</v>
       </c>
       <c r="M13" t="n">
-        <v>0.143</v>
+        <v>0.133</v>
       </c>
       <c r="N13" t="n">
-        <v>448.88</v>
+        <v>0.122</v>
       </c>
       <c r="O13" t="n">
-        <v>32.01</v>
+        <v>396.21</v>
       </c>
       <c r="P13" t="n">
-        <v>1354.04</v>
+        <v>17.76</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.355</v>
+        <v>1349.41</v>
       </c>
       <c r="R13" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="S13" t="n">
         <v>27.9</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3586,57 +3649,60 @@
         <v>6</v>
       </c>
       <c r="B14" t="n">
-        <v>86.67</v>
+        <v>39</v>
       </c>
       <c r="C14" t="n">
-        <v>5.93</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>49.14</v>
+        <v>76.86</v>
       </c>
       <c r="E14" t="n">
-        <v>-59.42</v>
+        <v>77.16</v>
       </c>
       <c r="F14" t="n">
-        <v>-5.06</v>
+        <v>-134</v>
       </c>
       <c r="G14" t="n">
-        <v>1.43</v>
+        <v>-7.51</v>
       </c>
       <c r="H14" t="n">
-        <v>-14.17</v>
+        <v>1.76</v>
       </c>
       <c r="I14" t="n">
-        <v>0.975</v>
+        <v>-14.92</v>
       </c>
       <c r="J14" t="n">
-        <v>4.72</v>
+        <v>1.032</v>
       </c>
       <c r="K14" t="n">
-        <v>0.5600000000000001</v>
+        <v>3.73</v>
       </c>
       <c r="L14" t="n">
-        <v>0.171</v>
+        <v>0.44</v>
       </c>
       <c r="M14" t="n">
-        <v>0.157</v>
+        <v>0.136</v>
       </c>
       <c r="N14" t="n">
-        <v>481.86</v>
+        <v>0.125</v>
       </c>
       <c r="O14" t="n">
-        <v>41.77</v>
+        <v>402.59</v>
       </c>
       <c r="P14" t="n">
-        <v>1318.12</v>
+        <v>19.34</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.397</v>
+        <v>1408.21</v>
       </c>
       <c r="R14" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="S14" t="n">
         <v>27.9</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3645,57 +3711,60 @@
         <v>7</v>
       </c>
       <c r="B15" t="n">
-        <v>101.11</v>
+        <v>45.5</v>
       </c>
       <c r="C15" t="n">
-        <v>5.09</v>
+        <v>8.34</v>
       </c>
       <c r="D15" t="n">
-        <v>38.42</v>
+        <v>71.17</v>
       </c>
       <c r="E15" t="n">
-        <v>-39.66</v>
+        <v>71.62</v>
       </c>
       <c r="F15" t="n">
-        <v>-4.5</v>
+        <v>-122.9</v>
       </c>
       <c r="G15" t="n">
-        <v>1.35</v>
+        <v>-7.12</v>
       </c>
       <c r="H15" t="n">
-        <v>-14.75</v>
+        <v>1.71</v>
       </c>
       <c r="I15" t="n">
-        <v>1.035</v>
+        <v>-14.7</v>
       </c>
       <c r="J15" t="n">
-        <v>5.33</v>
+        <v>1.013</v>
       </c>
       <c r="K15" t="n">
-        <v>0.63</v>
+        <v>3.82</v>
       </c>
       <c r="L15" t="n">
-        <v>0.193</v>
+        <v>0.45</v>
       </c>
       <c r="M15" t="n">
-        <v>0.177</v>
+        <v>0.139</v>
       </c>
       <c r="N15" t="n">
-        <v>529.16</v>
+        <v>0.127</v>
       </c>
       <c r="O15" t="n">
-        <v>56.79</v>
+        <v>409.57</v>
       </c>
       <c r="P15" t="n">
-        <v>1201.6</v>
+        <v>21.14</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.488</v>
+        <v>1366.75</v>
       </c>
       <c r="R15" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="S15" t="n">
         <v>27.9</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3704,57 +3773,60 @@
         <v>8</v>
       </c>
       <c r="B16" t="n">
-        <v>115.56</v>
+        <v>52</v>
       </c>
       <c r="C16" t="n">
-        <v>4.24</v>
+        <v>7.96</v>
       </c>
       <c r="D16" t="n">
-        <v>23.89</v>
+        <v>71.17</v>
       </c>
       <c r="E16" t="n">
-        <v>-20.98</v>
+        <v>71.62</v>
       </c>
       <c r="F16" t="n">
-        <v>-4.03</v>
+        <v>-112.1</v>
       </c>
       <c r="G16" t="n">
-        <v>1.27</v>
+        <v>-6.75</v>
       </c>
       <c r="H16" t="n">
-        <v>-14.95</v>
+        <v>1.66</v>
       </c>
       <c r="I16" t="n">
-        <v>1.087</v>
+        <v>-15.06</v>
       </c>
       <c r="J16" t="n">
-        <v>6.28</v>
+        <v>1.041</v>
       </c>
       <c r="K16" t="n">
-        <v>0.74</v>
+        <v>3.91</v>
       </c>
       <c r="L16" t="n">
-        <v>0.227</v>
+        <v>0.46</v>
       </c>
       <c r="M16" t="n">
-        <v>0.208</v>
+        <v>0.142</v>
       </c>
       <c r="N16" t="n">
-        <v>599.9</v>
+        <v>0.13</v>
       </c>
       <c r="O16" t="n">
-        <v>81.63</v>
+        <v>417.34</v>
       </c>
       <c r="P16" t="n">
-        <v>895.64</v>
+        <v>23.21</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.761</v>
+        <v>1432</v>
       </c>
       <c r="R16" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="S16" t="n">
         <v>27.9</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -3763,66 +3835,751 @@
         <v>9</v>
       </c>
       <c r="B17" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="D17" t="n">
+        <v>64.84999999999999</v>
+      </c>
+      <c r="E17" t="n">
+        <v>64.98</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-101.61</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-6.4</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-14.68</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.011</v>
+      </c>
+      <c r="K17" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="O17" t="n">
+        <v>426.09</v>
+      </c>
+      <c r="P17" t="n">
+        <v>25.59</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1364.33</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="S17" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T17" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B18" t="n">
+        <v>65</v>
+      </c>
+      <c r="C18" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>64.84999999999999</v>
+      </c>
+      <c r="E18" t="n">
+        <v>64.98</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-91.40000000000001</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-6.06</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-15.04</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="K18" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="O18" t="n">
+        <v>436.05</v>
+      </c>
+      <c r="P18" t="n">
+        <v>28.37</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1436.33</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="S18" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T18" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B19" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6.82</v>
+      </c>
+      <c r="D19" t="n">
+        <v>64.84999999999999</v>
+      </c>
+      <c r="E19" t="n">
+        <v>64.98</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-81.48</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-5.74</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-15.42</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="K19" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="O19" t="n">
+        <v>447.48</v>
+      </c>
+      <c r="P19" t="n">
+        <v>31.62</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1516.36</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="S19" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T19" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B20" t="n">
+        <v>78</v>
+      </c>
+      <c r="C20" t="n">
+        <v>6.44</v>
+      </c>
+      <c r="D20" t="n">
+        <v>57.66</v>
+      </c>
+      <c r="E20" t="n">
+        <v>58.34</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-71.84</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-5.44</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-14.95</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1.034</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="O20" t="n">
+        <v>460.7</v>
+      </c>
+      <c r="P20" t="n">
+        <v>35.46</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1441.69</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.344</v>
+      </c>
+      <c r="S20" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T20" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B21" t="n">
+        <v>84.5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>6.06</v>
+      </c>
+      <c r="D21" t="n">
+        <v>57.66</v>
+      </c>
+      <c r="E21" t="n">
+        <v>58.34</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-62.47</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-5.15</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-15.31</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.065</v>
+      </c>
+      <c r="K21" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.169</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="O21" t="n">
+        <v>476.1</v>
+      </c>
+      <c r="P21" t="n">
+        <v>40.04</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1532.09</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.337</v>
+      </c>
+      <c r="S21" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T21" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B22" t="n">
+        <v>91</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="D22" t="n">
+        <v>49.14</v>
+      </c>
+      <c r="E22" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-53.34</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-4.88</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-14.36</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.993</v>
+      </c>
+      <c r="K22" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.177</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="O22" t="n">
+        <v>494.16</v>
+      </c>
+      <c r="P22" t="n">
+        <v>45.58</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1386.45</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.389</v>
+      </c>
+      <c r="S22" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T22" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B23" t="n">
+        <v>97.5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>49.14</v>
+      </c>
+      <c r="E23" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-44.46</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-4.63</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-14.62</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="K23" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.187</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.171</v>
+      </c>
+      <c r="O23" t="n">
+        <v>515.5</v>
+      </c>
+      <c r="P23" t="n">
+        <v>52.35</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1485.85</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="S23" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T23" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B24" t="n">
+        <v>104</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="D24" t="n">
+        <v>38.42</v>
+      </c>
+      <c r="E24" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-35.81</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-4.4</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-14.83</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.047</v>
+      </c>
+      <c r="K24" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.199</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="O24" t="n">
+        <v>540.9299999999999</v>
+      </c>
+      <c r="P24" t="n">
+        <v>60.75</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1600.61</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.376</v>
+      </c>
+      <c r="S24" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T24" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B25" t="n">
+        <v>110.5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D25" t="n">
+        <v>38.42</v>
+      </c>
+      <c r="E25" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-27.38</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-4.18</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-14.95</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="K25" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.196</v>
+      </c>
+      <c r="O25" t="n">
+        <v>571.52</v>
+      </c>
+      <c r="P25" t="n">
+        <v>71.34999999999999</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1734.59</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.371</v>
+      </c>
+      <c r="S25" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T25" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B26" t="n">
+        <v>117</v>
+      </c>
+      <c r="C26" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D26" t="n">
+        <v>23.89</v>
+      </c>
+      <c r="E26" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-19.15</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-3.98</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-14.92</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="K26" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="O26" t="n">
+        <v>608.74</v>
+      </c>
+      <c r="P26" t="n">
+        <v>84.98</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1893.03</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.366</v>
+      </c>
+      <c r="S26" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T26" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B27" t="n">
+        <v>123.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="D27" t="n">
+        <v>23.89</v>
+      </c>
+      <c r="E27" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-11.11</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-14.61</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.098</v>
+      </c>
+      <c r="K27" t="n">
+        <v>7.03</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.255</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="O27" t="n">
+        <v>654.63</v>
+      </c>
+      <c r="P27" t="n">
+        <v>102.92</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2083.34</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="S27" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="T27" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B28" t="n">
         <v>130</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C28" t="n">
         <v>3.4</v>
       </c>
-      <c r="D17" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="E17" t="n">
+      <c r="D28" t="n">
+        <v>23.89</v>
+      </c>
+      <c r="E28" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="F28" t="n">
         <v>-3.24</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G28" t="n">
         <v>-3.64</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H28" t="n">
         <v>1.21</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I28" t="n">
         <v>-13.83</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J28" t="n">
         <v>1.085</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K28" t="n">
         <v>7.86</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L28" t="n">
         <v>0.93</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M28" t="n">
         <v>0.284</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N28" t="n">
         <v>0.26</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O28" t="n">
         <v>712.14</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P28" t="n">
         <v>127.21</v>
       </c>
-      <c r="P17" t="n">
-        <v>95.38</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="R17" t="n">
+      <c r="Q28" t="n">
+        <v>2316.18</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="S28" t="n">
         <v>27.9</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T28" t="n">
         <v>3.6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:S4"/>
-    <mergeCell ref="B5:S5"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="B5:T5"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I17">
+  <conditionalFormatting sqref="J3:J28">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3831,7 +4588,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L17">
+  <conditionalFormatting sqref="M3:M28">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3840,7 +4597,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M17">
+  <conditionalFormatting sqref="N3:N28">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3849,7 +4606,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q17">
+  <conditionalFormatting sqref="R3:R28">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3890,7 +4647,7 @@
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Ring Gerade t40</t>
+          <t>Ring Gerade t36</t>
         </is>
       </c>
     </row>
@@ -3901,7 +4658,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.086589733120714</v>
+        <v>1.097742484745861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>